<commit_message>
Domino I2S tile Rev. A: corrected ferrite beads to HH-1T2012-601
</commit_message>
<xml_diff>
--- a/Domino I2S/BOM/Domino I2S BOM.xlsx
+++ b/Domino I2S/BOM/Domino I2S BOM.xlsx
@@ -11,10 +11,10 @@
     <sheet name="Domino I2S Rev. A" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$15</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$14</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
@@ -24,19 +24,20 @@
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="100">
   <si>
     <t>Item</t>
   </si>
@@ -164,13 +165,16 @@
     <t>CERATECH</t>
   </si>
   <si>
+    <t>HH-1T2012-601</t>
+  </si>
+  <si>
     <t>FB0805</t>
   </si>
   <si>
     <t>FB1, FB2, FB3, FB4, FB5, FB6, FB7</t>
   </si>
   <si>
-    <t>FERRITE CHIP 120 OHM 800MA 0805</t>
+    <t>FERRITE CHIP 600 OHM 2500MA 0805</t>
   </si>
   <si>
     <t>ST-3538-050</t>
@@ -446,19 +450,19 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I22" activeCellId="0" pane="topLeft" sqref="I22"/>
+      <selection activeCell="F10" activeCellId="0" pane="topLeft" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.92941176470588"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.643137254902"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.7803921568627"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.7725490196078"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="40.9607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.2274509803922"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.0078431372549"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.95294117647059"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">
@@ -686,16 +690,16 @@
         <v>41</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="10">
@@ -706,22 +710,22 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D10" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="E10" s="0" t="s">
         <v>46</v>
       </c>
-      <c r="E10" s="0" t="s">
-        <v>45</v>
-      </c>
       <c r="F10" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="11">
@@ -732,22 +736,22 @@
         <v>2</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="D11" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="12">
@@ -758,22 +762,22 @@
         <v>0</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D12" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="13">
@@ -784,22 +788,22 @@
         <v>1</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="D13" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="14">
@@ -810,22 +814,22 @@
         <v>1</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D14" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="0" t="s">
         <v>61</v>
       </c>
-      <c r="E14" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="F14" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="15">
@@ -836,25 +840,25 @@
         <v>2</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="E15" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="0" t="s">
-        <v>64</v>
-      </c>
       <c r="F15" s="0" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="16">
+        <v>69</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="16">
       <c r="A16" s="0" t="n">
         <v>15</v>
       </c>
@@ -862,25 +866,25 @@
         <v>3</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="D16" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="17">
+        <v>74</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="17">
       <c r="A17" s="0" t="n">
         <v>16</v>
       </c>
@@ -888,25 +892,25 @@
         <v>2</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D17" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="18">
+        <v>78</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="18">
       <c r="A18" s="0" t="n">
         <v>17</v>
       </c>
@@ -914,25 +918,25 @@
         <v>1</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="D18" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="19">
+        <v>82</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="19">
       <c r="A19" s="0" t="n">
         <v>18</v>
       </c>
@@ -940,25 +944,25 @@
         <v>5</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D19" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="20">
+        <v>86</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="20">
       <c r="A20" s="0" t="n">
         <v>19</v>
       </c>
@@ -966,25 +970,25 @@
         <v>1</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D20" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="21">
+        <v>90</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="21">
       <c r="A21" s="0" t="n">
         <v>20</v>
       </c>
@@ -992,25 +996,25 @@
         <v>1</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D21" s="0" t="s">
         <v>10</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="12.1" outlineLevel="0" r="22">
+        <v>94</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.1" outlineLevel="0" r="22">
       <c r="A22" s="0" t="n">
         <v>21</v>
       </c>
@@ -1018,22 +1022,22 @@
         <v>1</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="D22" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="E22" s="0" t="s">
         <v>95</v>
       </c>
-      <c r="E22" s="0" t="s">
-        <v>94</v>
-      </c>
       <c r="F22" s="0" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Domino I2S tile Rev. B: made board multiple of 100 mils Cleaned up silkscreen made +5V trace wider Aligned some components
</commit_message>
<xml_diff>
--- a/Domino I2S/BOM/Domino I2S BOM.xlsx
+++ b/Domino I2S/BOM/Domino I2S BOM.xlsx
@@ -8,29 +8,30 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino I2S Rev. A" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino I2S Rev. B" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. A'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -454,15 +455,14 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.95686274509804"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.7882352941176"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="31.9372549019608"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="26.9058823529412"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.1607843137255"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.5450980392157"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.1333333333333"/>
-    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="9"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.043137254902"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>

<commit_message>
Domino I2S Rev. C: changed silkscreen font ratio to 20%
</commit_message>
<xml_diff>
--- a/Domino I2S/BOM/Domino I2S BOM.xlsx
+++ b/Domino I2S/BOM/Domino I2S BOM.xlsx
@@ -8,30 +8,31 @@
     <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="77" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Domino I2S Rev. B" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Domino I2S Rev. C" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$22</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$15</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$14</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$9</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. B'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$22</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$15</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$14</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$9</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$1</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm.Print_Area_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0_0" vbProcedure="false">'Domino I2S Rev. C'!$A$1:$I$1</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
 </workbook>
@@ -455,14 +456,15 @@
     </sheetView>
   </sheetViews>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="4.9843137254902"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.043137254902"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="28.9333333333333"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.0980392156863"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.043137254902"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.3686274509804"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="63.8627450980392"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.2627450980392"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="0" width="5.01176470588235"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="27.1764705882353"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="29.078431372549"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="32.2627450980392"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="27.1764705882353"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="41.5764705882353"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="64.1803921568628"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="25.3882352941176"/>
+    <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.54509803921569"/>
   </cols>
   <sheetData>
     <row collapsed="false" customFormat="false" customHeight="true" hidden="false" ht="12.65" outlineLevel="0" r="1">

</xml_diff>